<commit_message>
Added: 	Meeting 3 Minutes 	Meeting 3 Evidence (Dicsord ScreenShot) 	Updated Progress and Estimation Spreadsheet 	Cleaned Up Directories
</commit_message>
<xml_diff>
--- a/Progress&Estimations.xlsx
+++ b/Progress&Estimations.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="33">
   <si>
     <t xml:space="preserve">Sprint 1 - Initial Task Allocation</t>
   </si>
@@ -31,12 +31,12 @@
     <t xml:space="preserve">Friday</t>
   </si>
   <si>
+    <t xml:space="preserve">Ideal Task Progress</t>
+  </si>
+  <si>
     <t xml:space="preserve">Task Progress Daily Estimate</t>
   </si>
   <si>
-    <t xml:space="preserve">Ideal Task Progress</t>
-  </si>
-  <si>
     <t xml:space="preserve">Shan</t>
   </si>
   <si>
@@ -103,10 +103,22 @@
     <t xml:space="preserve">Meeting Attendance</t>
   </si>
   <si>
+    <t xml:space="preserve">Mtg1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mtg2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mtg3</t>
+  </si>
+  <si>
     <t xml:space="preserve">Abset</t>
   </si>
   <si>
     <t xml:space="preserve">Present</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Absent</t>
   </si>
 </sst>
 </file>
@@ -325,7 +337,7 @@
   <dimension ref="A1:AJ37"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AI58" activeCellId="0" sqref="AH58:AI62"/>
+      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -468,6 +480,21 @@
       <c r="A6" s="0" t="s">
         <v>5</v>
       </c>
+      <c r="B6" s="0" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="L6" s="6"/>
       <c r="N6" s="7"/>
       <c r="P6" s="0" t="s">
@@ -477,6 +504,12 @@
       <c r="AB6" s="0" t="s">
         <v>7</v>
       </c>
+      <c r="AD6" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="AE6" s="0" t="n">
+        <v>80</v>
+      </c>
       <c r="AJ6" s="8"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -487,6 +520,12 @@
         <v>2.5</v>
       </c>
       <c r="E7" s="0" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="G7" s="0" t="n">
         <v>2.5</v>
       </c>
       <c r="L7" s="6"/>
@@ -498,6 +537,12 @@
       <c r="AB7" s="0" t="s">
         <v>10</v>
       </c>
+      <c r="AD7" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="AE7" s="0" t="n">
+        <v>60</v>
+      </c>
       <c r="AJ7" s="8"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -508,6 +553,12 @@
         <v>2.5</v>
       </c>
       <c r="E8" s="0" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="G8" s="0" t="n">
         <v>2.5</v>
       </c>
       <c r="L8" s="6"/>
@@ -519,17 +570,32 @@
       <c r="AB8" s="0" t="s">
         <v>13</v>
       </c>
+      <c r="AD8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE8" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="AJ8" s="8"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>14</v>
       </c>
+      <c r="B9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="D9" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E9" s="0" t="n">
         <v>1</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>3</v>
       </c>
       <c r="L9" s="6"/>
       <c r="N9" s="7"/>
@@ -540,17 +606,32 @@
       <c r="AB9" s="0" t="s">
         <v>16</v>
       </c>
+      <c r="AD9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE9" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="AJ9" s="8"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>17</v>
       </c>
+      <c r="B10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="D10" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E10" s="0" t="n">
         <v>1</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>3</v>
       </c>
       <c r="L10" s="6"/>
       <c r="N10" s="7"/>
@@ -564,30 +645,57 @@
       <c r="AB10" s="0" t="s">
         <v>20</v>
       </c>
+      <c r="AD10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE10" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="AJ10" s="8"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>21</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="L11" s="6"/>
       <c r="N11" s="7"/>
       <c r="P11" s="0" t="s">
         <v>22</v>
       </c>
+      <c r="X11" s="0" t="n">
+        <v>75</v>
+      </c>
+      <c r="Y11" s="0" t="n">
+        <v>100</v>
+      </c>
       <c r="Z11" s="8"/>
       <c r="AB11" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="AF11" s="9" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="AH11" s="9" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="AI11" s="9" t="n">
-        <v>1</v>
-      </c>
+      <c r="AD11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="AE11" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="AF11" s="9"/>
+      <c r="AH11" s="9"/>
+      <c r="AI11" s="9"/>
       <c r="AJ11" s="8"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -665,6 +773,15 @@
       <c r="A22" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="B22" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="G22" s="0" t="s">
+        <v>29</v>
+      </c>
       <c r="I22" s="0" t="s">
         <v>2</v>
       </c>
@@ -712,10 +829,13 @@
         <v>5</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
+      </c>
+      <c r="G25" s="0" t="s">
+        <v>31</v>
       </c>
       <c r="L25" s="6"/>
     </row>
@@ -724,10 +844,13 @@
         <v>8</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
+      </c>
+      <c r="G26" s="0" t="s">
+        <v>31</v>
       </c>
       <c r="L26" s="6"/>
     </row>
@@ -736,10 +859,13 @@
         <v>11</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
+      </c>
+      <c r="G27" s="0" t="s">
+        <v>31</v>
       </c>
       <c r="L27" s="6"/>
     </row>
@@ -747,8 +873,14 @@
       <c r="A28" s="0" t="s">
         <v>14</v>
       </c>
+      <c r="B28" s="0" t="s">
+        <v>31</v>
+      </c>
       <c r="E28" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
+      </c>
+      <c r="G28" s="0" t="s">
+        <v>31</v>
       </c>
       <c r="L28" s="6"/>
     </row>
@@ -756,14 +888,29 @@
       <c r="A29" s="0" t="s">
         <v>17</v>
       </c>
+      <c r="B29" s="0" t="s">
+        <v>31</v>
+      </c>
       <c r="E29" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
+      </c>
+      <c r="G29" s="0" t="s">
+        <v>31</v>
       </c>
       <c r="L29" s="6"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
         <v>21</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E30" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="G30" s="0" t="s">
+        <v>31</v>
       </c>
       <c r="L30" s="6"/>
     </row>

</xml_diff>

<commit_message>
Added Meeting #4 Minutes Added Meeting #4 Proof Updated Progress&Estimations.xlsx
</commit_message>
<xml_diff>
--- a/Progress&Estimations.xlsx
+++ b/Progress&Estimations.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="34">
   <si>
     <t xml:space="preserve">Sprint 1 - Initial Task Allocation</t>
   </si>
@@ -110,6 +110,9 @@
   </si>
   <si>
     <t xml:space="preserve">Mtg3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mtg 4</t>
   </si>
   <si>
     <t xml:space="preserve">Abset</t>
@@ -336,8 +339,8 @@
   </sheetPr>
   <dimension ref="A1:AJ37"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AG27" activeCellId="0" sqref="AG27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -495,6 +498,12 @@
       <c r="F6" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="G6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>0.5</v>
+      </c>
       <c r="L6" s="6"/>
       <c r="N6" s="7"/>
       <c r="P6" s="0" t="s">
@@ -510,6 +519,9 @@
       <c r="AE6" s="0" t="n">
         <v>80</v>
       </c>
+      <c r="AF6" s="0" t="n">
+        <v>80</v>
+      </c>
       <c r="AJ6" s="8"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -527,6 +539,9 @@
       </c>
       <c r="G7" s="0" t="n">
         <v>2.5</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>0.5</v>
       </c>
       <c r="L7" s="6"/>
       <c r="N7" s="7"/>
@@ -543,6 +558,9 @@
       <c r="AE7" s="0" t="n">
         <v>60</v>
       </c>
+      <c r="AF7" s="0" t="n">
+        <v>80</v>
+      </c>
       <c r="AJ7" s="8"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -560,6 +578,9 @@
       </c>
       <c r="G8" s="0" t="n">
         <v>2.5</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <v>0.5</v>
       </c>
       <c r="L8" s="6"/>
       <c r="N8" s="7"/>
@@ -576,6 +597,9 @@
       <c r="AE8" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="AF8" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="AJ8" s="8"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -596,6 +620,12 @@
       </c>
       <c r="F9" s="0" t="n">
         <v>3</v>
+      </c>
+      <c r="G9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="L9" s="6"/>
       <c r="N9" s="7"/>
@@ -612,6 +642,9 @@
       <c r="AE9" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="AF9" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="AJ9" s="8"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -632,6 +665,12 @@
       </c>
       <c r="F10" s="0" t="n">
         <v>3</v>
+      </c>
+      <c r="G10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="L10" s="6"/>
       <c r="N10" s="7"/>
@@ -651,6 +690,9 @@
       <c r="AE10" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="AF10" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="AJ10" s="8"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -671,6 +713,12 @@
       </c>
       <c r="F11" s="0" t="n">
         <v>0</v>
+      </c>
+      <c r="G11" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="H11" s="0" t="n">
+        <v>1.5</v>
       </c>
       <c r="L11" s="6"/>
       <c r="N11" s="7"/>
@@ -693,7 +741,9 @@
       <c r="AE11" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="AF11" s="9"/>
+      <c r="AF11" s="9" t="n">
+        <v>0.2</v>
+      </c>
       <c r="AH11" s="9"/>
       <c r="AI11" s="9"/>
       <c r="AJ11" s="8"/>
@@ -782,6 +832,9 @@
       <c r="G22" s="0" t="s">
         <v>29</v>
       </c>
+      <c r="H22" s="0" t="s">
+        <v>30</v>
+      </c>
       <c r="I22" s="0" t="s">
         <v>2</v>
       </c>
@@ -829,13 +882,16 @@
         <v>5</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
+      </c>
+      <c r="H25" s="0" t="s">
+        <v>32</v>
       </c>
       <c r="L25" s="6"/>
     </row>
@@ -844,13 +900,16 @@
         <v>8</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
+      </c>
+      <c r="H26" s="0" t="s">
+        <v>32</v>
       </c>
       <c r="L26" s="6"/>
     </row>
@@ -859,13 +918,16 @@
         <v>11</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
+      </c>
+      <c r="H27" s="0" t="s">
+        <v>32</v>
       </c>
       <c r="L27" s="6"/>
     </row>
@@ -874,13 +936,16 @@
         <v>14</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
+      </c>
+      <c r="H28" s="0" t="s">
+        <v>32</v>
       </c>
       <c r="L28" s="6"/>
     </row>
@@ -889,13 +954,16 @@
         <v>17</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
+      </c>
+      <c r="H29" s="0" t="s">
+        <v>32</v>
       </c>
       <c r="L29" s="6"/>
     </row>
@@ -904,13 +972,16 @@
         <v>21</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
+      </c>
+      <c r="H30" s="0" t="s">
+        <v>32</v>
       </c>
       <c r="L30" s="6"/>
     </row>

</xml_diff>

<commit_message>
scrum meeting 2 evidence, minutes, updates, etc.
</commit_message>
<xml_diff>
--- a/Progress&Estimations.xlsx
+++ b/Progress&Estimations.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="53">
   <si>
     <t xml:space="preserve">Sprint 1 - Initial Task Allocation</t>
   </si>
@@ -1136,16 +1136,16 @@
   </sheetPr>
   <dimension ref="A1:AN37"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K28" activeCellId="0" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="15.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="15.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="7" style="0" width="8.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="11.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="11" style="0" width="8.53"/>
@@ -1328,6 +1328,12 @@
       <c r="G7" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="H7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>5</v>
+      </c>
       <c r="P7" s="6"/>
       <c r="R7" s="7"/>
       <c r="AD7" s="8"/>
@@ -1355,6 +1361,9 @@
       <c r="G8" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="I8" s="0" t="n">
+        <v>5</v>
+      </c>
       <c r="P8" s="6"/>
       <c r="R8" s="7"/>
       <c r="AD8" s="8"/>
@@ -1370,6 +1379,9 @@
       <c r="G9" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="I9" s="0" t="n">
+        <v>3</v>
+      </c>
       <c r="P9" s="6"/>
       <c r="R9" s="7"/>
       <c r="AD9" s="8"/>
@@ -1388,6 +1400,9 @@
       <c r="G10" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="I10" s="0" t="n">
+        <v>3</v>
+      </c>
       <c r="P10" s="6"/>
       <c r="R10" s="7"/>
       <c r="AD10" s="8"/>
@@ -1396,6 +1411,9 @@
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>28</v>
+      </c>
+      <c r="I11" s="0" t="n">
+        <v>1.5</v>
       </c>
       <c r="P11" s="6"/>
       <c r="R11" s="7"/>
@@ -1514,6 +1532,9 @@
       <c r="H25" s="0" t="s">
         <v>52</v>
       </c>
+      <c r="I25" s="0" t="s">
+        <v>52</v>
+      </c>
       <c r="P25" s="6"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1529,6 +1550,9 @@
       <c r="H26" s="0" t="s">
         <v>52</v>
       </c>
+      <c r="I26" s="0" t="s">
+        <v>52</v>
+      </c>
       <c r="P26" s="6"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1544,6 +1568,9 @@
       <c r="H27" s="0" t="s">
         <v>52</v>
       </c>
+      <c r="I27" s="0" t="s">
+        <v>52</v>
+      </c>
       <c r="P27" s="6"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1559,6 +1586,9 @@
       <c r="H28" s="0" t="s">
         <v>52</v>
       </c>
+      <c r="I28" s="0" t="s">
+        <v>52</v>
+      </c>
       <c r="P28" s="6"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1574,6 +1604,9 @@
       <c r="H29" s="0" t="s">
         <v>52</v>
       </c>
+      <c r="I29" s="0" t="s">
+        <v>52</v>
+      </c>
       <c r="P29" s="6"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1587,6 +1620,9 @@
         <v>52</v>
       </c>
       <c r="H30" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="I30" s="0" t="s">
         <v>52</v>
       </c>
       <c r="P30" s="6"/>

</xml_diff>